<commit_message>
Frequenztabellen aufgeteilt für Lautsprecher
</commit_message>
<xml_diff>
--- a/Versuch3_Messungen/Versuch3_Frequenztabelle.xlsx
+++ b/Versuch3_Messungen/Versuch3_Frequenztabelle.xlsx
@@ -1,33 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\al871sch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSS\SSS_aufgaben\Versuch3_Messungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932C5893-31A3-4F0D-8E93-6C77C7E1EE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCACBC65-11CC-4D97-9B68-1937F928E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{178A48E5-6DE8-4865-8338-E456A673EB5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{178A48E5-6DE8-4865-8338-E456A673EB5A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lautsprecher1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lautsprecher2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -101,9 +93,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9BABFD-853F-4193-B3A1-5B58E2B93DC8}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +407,7 @@
     <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -428,20 +420,8 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -454,20 +434,8 @@
       <c r="D2">
         <v>5.532</v>
       </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>1.5</v>
-      </c>
-      <c r="H2">
-        <v>14.72</v>
-      </c>
-      <c r="I2">
-        <v>3.8450000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -480,20 +448,8 @@
       <c r="D3">
         <v>4.5389999999999997</v>
       </c>
-      <c r="F3">
-        <v>200</v>
-      </c>
-      <c r="G3">
-        <v>1.5</v>
-      </c>
-      <c r="H3">
-        <v>31.18</v>
-      </c>
-      <c r="I3">
-        <v>3.1230000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
@@ -506,20 +462,8 @@
       <c r="D4">
         <v>0.223</v>
       </c>
-      <c r="F4">
-        <v>300</v>
-      </c>
-      <c r="G4">
-        <v>1.5</v>
-      </c>
-      <c r="H4">
-        <v>44.17</v>
-      </c>
-      <c r="I4">
-        <v>2.4020000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
@@ -532,20 +476,8 @@
       <c r="D5">
         <v>0.30599999999999999</v>
       </c>
-      <c r="F5">
-        <v>400</v>
-      </c>
-      <c r="G5">
-        <v>1.4830000000000001</v>
-      </c>
-      <c r="H5">
-        <v>80.540000000000006</v>
-      </c>
-      <c r="I5">
-        <v>1.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -558,20 +490,8 @@
       <c r="D6">
         <v>0.30199999999999999</v>
       </c>
-      <c r="F6">
-        <v>500</v>
-      </c>
-      <c r="G6">
-        <v>1.5</v>
-      </c>
-      <c r="H6">
-        <v>172.3</v>
-      </c>
-      <c r="I6">
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>700</v>
       </c>
@@ -584,20 +504,8 @@
       <c r="D7">
         <v>0.24299999999999999</v>
       </c>
-      <c r="F7">
-        <v>700</v>
-      </c>
-      <c r="G7">
-        <v>1.5</v>
-      </c>
-      <c r="H7">
-        <v>70.14</v>
-      </c>
-      <c r="I7">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>850</v>
       </c>
@@ -610,20 +518,8 @@
       <c r="D8">
         <v>0.192</v>
       </c>
-      <c r="F8">
-        <v>850</v>
-      </c>
-      <c r="G8">
-        <v>1.5</v>
-      </c>
-      <c r="H8">
-        <v>49.36</v>
-      </c>
-      <c r="I8">
-        <v>0.25600000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000</v>
       </c>
@@ -636,20 +532,8 @@
       <c r="D9">
         <v>0.17899999999999999</v>
       </c>
-      <c r="F9">
-        <v>1000</v>
-      </c>
-      <c r="G9">
-        <v>1.5</v>
-      </c>
-      <c r="H9">
-        <v>42.43</v>
-      </c>
-      <c r="I9">
-        <v>0.22700000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1200</v>
       </c>
@@ -662,20 +546,8 @@
       <c r="D10">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F10">
-        <v>1200</v>
-      </c>
-      <c r="G10">
-        <v>1.5</v>
-      </c>
-      <c r="H10">
-        <v>32.04</v>
-      </c>
-      <c r="I10">
-        <v>0.192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1500</v>
       </c>
@@ -688,20 +560,8 @@
       <c r="D11">
         <v>0.16</v>
       </c>
-      <c r="F11">
-        <v>1500</v>
-      </c>
-      <c r="G11">
-        <v>1.5</v>
-      </c>
-      <c r="H11">
-        <v>37.24</v>
-      </c>
-      <c r="I11">
-        <v>0.18099999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1700</v>
       </c>
@@ -714,20 +574,8 @@
       <c r="D12">
         <v>0.155</v>
       </c>
-      <c r="F12">
-        <v>1700</v>
-      </c>
-      <c r="G12">
-        <v>1.5</v>
-      </c>
-      <c r="H12">
-        <v>33.770000000000003</v>
-      </c>
-      <c r="I12">
-        <v>0.16300000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -740,20 +588,8 @@
       <c r="D13">
         <v>0.152</v>
       </c>
-      <c r="F13">
-        <v>2000</v>
-      </c>
-      <c r="G13">
-        <v>1.5</v>
-      </c>
-      <c r="H13">
-        <v>34.64</v>
-      </c>
-      <c r="I13">
-        <v>0.155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3000</v>
       </c>
@@ -766,20 +602,8 @@
       <c r="D14">
         <v>0.15</v>
       </c>
-      <c r="F14">
-        <v>3000</v>
-      </c>
-      <c r="G14">
-        <v>1.5</v>
-      </c>
-      <c r="H14">
-        <v>42.43</v>
-      </c>
-      <c r="I14">
-        <v>0.13900000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4000</v>
       </c>
@@ -792,20 +616,8 @@
       <c r="D15">
         <v>0.14399999999999999</v>
       </c>
-      <c r="F15">
-        <v>4000</v>
-      </c>
-      <c r="G15">
-        <v>1.5</v>
-      </c>
-      <c r="H15">
-        <v>36.369999999999997</v>
-      </c>
-      <c r="I15">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -818,20 +630,8 @@
       <c r="D16">
         <v>0.152</v>
       </c>
-      <c r="F16">
-        <v>5000</v>
-      </c>
-      <c r="G16">
-        <v>1.5</v>
-      </c>
-      <c r="H16">
-        <v>49.36</v>
-      </c>
-      <c r="I16">
-        <v>0.16600000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6000</v>
       </c>
@@ -844,20 +644,8 @@
       <c r="D17">
         <v>0.123</v>
       </c>
-      <c r="F17">
-        <v>6000</v>
-      </c>
-      <c r="G17">
-        <v>1.5</v>
-      </c>
-      <c r="H17">
-        <v>17.32</v>
-      </c>
-      <c r="I17">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10000</v>
       </c>
@@ -870,16 +658,271 @@
       <c r="D18">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="F18">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A07335-3B21-42F3-84CE-739C3F9495B7}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <v>14.72</v>
+      </c>
+      <c r="D2">
+        <v>3.8450000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>31.18</v>
+      </c>
+      <c r="D3">
+        <v>3.1230000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>44.17</v>
+      </c>
+      <c r="D4">
+        <v>2.4020000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>400</v>
+      </c>
+      <c r="B5">
+        <v>1.4830000000000001</v>
+      </c>
+      <c r="C5">
+        <v>80.540000000000006</v>
+      </c>
+      <c r="D5">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>172.3</v>
+      </c>
+      <c r="D6">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>700</v>
+      </c>
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="C7">
+        <v>70.14</v>
+      </c>
+      <c r="D7">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>850</v>
+      </c>
+      <c r="B8">
+        <v>1.5</v>
+      </c>
+      <c r="C8">
+        <v>49.36</v>
+      </c>
+      <c r="D8">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>1.5</v>
+      </c>
+      <c r="C9">
+        <v>42.43</v>
+      </c>
+      <c r="D9">
+        <v>0.22700000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1200</v>
+      </c>
+      <c r="B10">
+        <v>1.5</v>
+      </c>
+      <c r="C10">
+        <v>32.04</v>
+      </c>
+      <c r="D10">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1500</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="C11">
+        <v>37.24</v>
+      </c>
+      <c r="D11">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1700</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
+      <c r="C12">
+        <v>33.770000000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.16300000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2000</v>
+      </c>
+      <c r="B13">
+        <v>1.5</v>
+      </c>
+      <c r="C13">
+        <v>34.64</v>
+      </c>
+      <c r="D13">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3000</v>
+      </c>
+      <c r="B14">
+        <v>1.5</v>
+      </c>
+      <c r="C14">
+        <v>42.43</v>
+      </c>
+      <c r="D14">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4000</v>
+      </c>
+      <c r="B15">
+        <v>1.5</v>
+      </c>
+      <c r="C15">
+        <v>36.369999999999997</v>
+      </c>
+      <c r="D15">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5000</v>
+      </c>
+      <c r="B16">
+        <v>1.5</v>
+      </c>
+      <c r="C16">
+        <v>49.36</v>
+      </c>
+      <c r="D16">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6000</v>
+      </c>
+      <c r="B17">
+        <v>1.5</v>
+      </c>
+      <c r="C17">
+        <v>17.32</v>
+      </c>
+      <c r="D17">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>10000</v>
       </c>
-      <c r="G18">
-        <v>1.5</v>
-      </c>
-      <c r="H18">
+      <c r="B18">
+        <v>1.5</v>
+      </c>
+      <c r="C18">
         <v>24.25</v>
       </c>
-      <c r="I18">
+      <c r="D18">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Versuch 5 Notebook Dateien hinzugefügt
</commit_message>
<xml_diff>
--- a/Versuch3_Messungen/Versuch3_Frequenztabelle.xlsx
+++ b/Versuch3_Messungen/Versuch3_Frequenztabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSS\SSS_aufgaben\Versuch3_Messungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCACBC65-11CC-4D97-9B68-1937F928E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7AA78D-9488-41CB-8132-E204C4E173BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{178A48E5-6DE8-4865-8338-E456A673EB5A}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{178A48E5-6DE8-4865-8338-E456A673EB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Lautsprecher1" sheetId="1" r:id="rId1"/>
@@ -391,23 +391,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9BABFD-853F-4193-B3A1-5B58E2B93DC8}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -435,7 +435,7 @@
         <v>5.532</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>200</v>
       </c>
@@ -449,7 +449,7 @@
         <v>4.5389999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>300</v>
       </c>
@@ -463,7 +463,7 @@
         <v>0.223</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>400</v>
       </c>
@@ -477,7 +477,7 @@
         <v>0.30599999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>500</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0.30199999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>700</v>
       </c>
@@ -505,7 +505,7 @@
         <v>0.24299999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>850</v>
       </c>
@@ -519,7 +519,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1000</v>
       </c>
@@ -533,7 +533,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1200</v>
       </c>
@@ -547,7 +547,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1500</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1700</v>
       </c>
@@ -575,7 +575,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -589,7 +589,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3000</v>
       </c>
@@ -603,7 +603,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4000</v>
       </c>
@@ -617,7 +617,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -631,7 +631,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>6000</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>10000</v>
       </c>
@@ -668,13 +668,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A07335-3B21-42F3-84CE-739C3F9495B7}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -688,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -702,7 +706,7 @@
         <v>3.8450000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>200</v>
       </c>
@@ -716,7 +720,7 @@
         <v>3.1230000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>300</v>
       </c>
@@ -730,7 +734,7 @@
         <v>2.4020000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>400</v>
       </c>
@@ -744,7 +748,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>500</v>
       </c>
@@ -758,7 +762,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>700</v>
       </c>
@@ -772,7 +776,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>850</v>
       </c>
@@ -786,7 +790,7 @@
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1000</v>
       </c>
@@ -800,7 +804,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1200</v>
       </c>
@@ -814,7 +818,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1500</v>
       </c>
@@ -828,7 +832,7 @@
         <v>0.18099999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1700</v>
       </c>
@@ -842,7 +846,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -856,7 +860,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3000</v>
       </c>
@@ -870,7 +874,7 @@
         <v>0.13900000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4000</v>
       </c>
@@ -884,7 +888,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -898,7 +902,7 @@
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>6000</v>
       </c>
@@ -912,7 +916,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>10000</v>
       </c>

</xml_diff>